<commit_message>
Adding RE2.2 Generic DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Intent_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Intent_JS.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -479,24 +479,6 @@
 validate4
 {
 validate_App_Launched_Device=com.android.gallery3d
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Intent JS Test
-};
-validate3
-{
-validate_OldText_Exists=VT328_29
-};
-validate4
-{
-validate_App_Launched_Device=com.android.browser
 };</t>
   </si>
   <si>
@@ -1260,22 +1242,6 @@
 validate1;
 link_Click(intent_test_link);
 validate2;
-SelectTestToRun(VT328_29_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(5);
-validate4;
-SwitchApp(NATIVE_APP);
-wait(2);
-CheckUITextContains(Google);
-press_Key(Back);</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(intent_test_link);
-validate2;
 SelectTestToRun(VT328_45_string);
 ClickRunTest(runtest_top_xpath);
 validate3;
@@ -1311,6 +1277,44 @@
 ClickRunTest(runtest_bottom_xpath);
 wait(5);
 validate4;
+press_Key(Back);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Intent JS Test
+};
+validate3
+{
+validate_OldText_Exists=VT328_29
+};
+validate4
+{
+validate_App_Launched_Device=com.android.browser
+};
+validate5
+{
+validate_CompareEditText=0,google
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(intent_test_link);
+validate2;
+SelectTestToRun(VT328_29_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+validate4;
+SwitchApp(NATIVE_APP);
+wait(2);
+validate5;
 press_Key(Back);</t>
   </si>
 </sst>
@@ -1805,7 +1809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1865,13 +1869,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="9">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9" t="s">
@@ -2033,10 +2037,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2060,10 +2064,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -2114,10 +2118,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -2168,10 +2172,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -2195,10 +2199,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -2225,7 +2229,7 @@
         <v>28</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -2249,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>55</v>
@@ -2276,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>56</v>
@@ -2303,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>57</v>
@@ -2330,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>58</v>
@@ -2357,7 +2361,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>59</v>
@@ -2384,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>60</v>
@@ -2393,7 +2397,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11" ht="204">
+    <row r="22" spans="1:11" ht="255">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -2411,10 +2415,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -2438,10 +2442,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -2465,10 +2469,10 @@
         <v>1</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -2492,10 +2496,10 @@
         <v>1</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -2519,10 +2523,10 @@
         <v>1</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -2546,10 +2550,10 @@
         <v>1</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -2573,10 +2577,10 @@
         <v>1</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -2600,10 +2604,10 @@
         <v>1</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -2621,16 +2625,16 @@
         <v>10</v>
       </c>
       <c r="E30" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="9">
+        <v>1</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="9">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9" t="s">
+      <c r="H30" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="229.5">
@@ -2645,14 +2649,14 @@
         <v>10</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="204">
@@ -2667,14 +2671,14 @@
         <v>10</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="165.75">
@@ -2695,10 +2699,10 @@
         <v>1</v>
       </c>
       <c r="G33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="165.75">
@@ -2713,16 +2717,16 @@
         <v>10</v>
       </c>
       <c r="E34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F34" s="9">
-        <v>1</v>
-      </c>
-      <c r="G34" s="9" t="s">
+      <c r="H34" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="216.75">
@@ -2737,16 +2741,16 @@
         <v>10</v>
       </c>
       <c r="E35" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F35" s="9">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9" t="s">
+      <c r="H35" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="165.75">
@@ -2761,16 +2765,16 @@
         <v>10</v>
       </c>
       <c r="E36" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="9">
+        <v>1</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F36" s="9">
-        <v>1</v>
-      </c>
-      <c r="G36" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="165.75">
@@ -2785,16 +2789,16 @@
         <v>10</v>
       </c>
       <c r="E37" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="9">
+        <v>1</v>
+      </c>
+      <c r="G37" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F37" s="9">
-        <v>1</v>
-      </c>
-      <c r="G37" s="9" t="s">
+      <c r="H37" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>